<commit_message>
Atualização automática de VIAMAO.xlsx
</commit_message>
<xml_diff>
--- a/VIAMAO.xlsx
+++ b/VIAMAO.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\gera-fichas\Comarcas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2ADE434E-9DFD-4AA6-B8B8-DA60CED56C7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{46BCFA6E-64E2-40E4-ACFB-6648FF3743EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Paineis DARQ" sheetId="8" r:id="rId1"/>
+    <sheet name="Paineis DARQ" sheetId="9" r:id="rId1"/>
     <sheet name="DESFAZIMENTOS" sheetId="1" r:id="rId2"/>
     <sheet name="MATERIAIS-FORNECIDOS" sheetId="2" r:id="rId3"/>
     <sheet name="DATA-LIMITE-REQUISICOES" sheetId="3" r:id="rId4"/>
@@ -21,13 +21,14 @@
     <sheet name="TCA" sheetId="5" r:id="rId6"/>
     <sheet name="Recolhimento x Eliminacao" sheetId="6" r:id="rId7"/>
     <sheet name="Desarquivamentos Pendentes" sheetId="7" r:id="rId8"/>
+    <sheet name="DGC" sheetId="8" r:id="rId9"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1019" uniqueCount="355">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1025" uniqueCount="359">
   <si>
     <t>COMARCA</t>
   </si>
@@ -1092,6 +1093,18 @@
   </si>
   <si>
     <t>%</t>
+  </si>
+  <si>
+    <t>TEMÁTICA</t>
+  </si>
+  <si>
+    <t>PROBLEMA</t>
+  </si>
+  <si>
+    <t>MAOBRAS/MATIC</t>
+  </si>
+  <si>
+    <t>Muitas correções do ateste.</t>
   </si>
 </sst>
 </file>
@@ -1102,7 +1115,7 @@
     <numFmt numFmtId="44" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="165" formatCode="&quot; &quot;mmmm&quot; / &quot;yyyy"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1155,6 +1168,19 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+    </font>
+    <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -1169,7 +1195,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1216,6 +1242,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFB7E1CD"/>
         <bgColor rgb="FFB7E1CD"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD9D9D9"/>
+        <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
     <fill>
@@ -1288,9 +1320,9 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1380,12 +1412,16 @@
     <xf numFmtId="3" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 3" xfId="1" xr:uid="{36D35E2B-43F8-4ED5-8E9D-421ABB8392D7}"/>
+    <cellStyle name="Normal 3" xfId="1" xr:uid="{8116AE77-634C-4578-A388-741375B5436E}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1415,10 +1451,10 @@
         <xdr:cNvPr id="2" name="Chart1" title="Gráfico">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{423B684F-7FD0-47FF-9496-2FF9906199EA}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E24F23D0-B73D-4752-A58B-528329BF6D4C}"/>
             </a:ext>
             <a:ext uri="GoogleSheetsCustomDataVersion1">
-              <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="" pictureOfChart="1"/>
+              <go:sheetsCustomData xmlns="" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" xmlns:go="http://customooxmlschemas.google.com/" pictureOfChart="1"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1456,7 +1492,7 @@
         <xdr:cNvPr id="3" name="Shape 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D1A228E2-C7FE-40AB-AC6A-1AA4375DD9A2}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4220DE21-6B59-477D-AAEF-399F8F8D012D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1519,7 +1555,7 @@
         <xdr:cNvPr id="4" name="Shape 2" title="Desenho">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EF32B193-C84A-407A-944F-6854FC38D9F5}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E49BE186-98DC-48DD-89DC-F8265D145D4F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1538,7 +1574,7 @@
           <xdr:cNvPr id="5" name="Shape 4">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7BD1BD71-F65F-427B-B65A-976B0BC0814C}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E2C6A81A-259C-679A-8E68-ADEF4A2C44A8}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1587,7 +1623,7 @@
           <xdr:cNvPr id="6" name="Shape 5">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{545D80C0-4218-AF54-F8F7-9FF2ED637BBA}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{53D4BA9B-5B45-36FA-66C8-4D301F7B63C2}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1606,7 +1642,7 @@
             <xdr:cNvPr id="7" name="Shape 6">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DED6C0FD-A350-0F9D-EE01-527ECD17FE04}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4DC94C04-A399-7DF1-6650-9864D2D7F38D}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1637,7 +1673,7 @@
             <xdr:cNvPr id="8" name="Shape 7">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C751C477-22DD-5175-8C13-5D1D4618A34D}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{52A08ABE-38E4-86F0-2FCC-2020A5C2D854}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1668,7 +1704,7 @@
             <xdr:cNvPr id="9" name="Shape 8">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{33957269-F45E-3B9E-BFB5-3985B1AA56FE}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9816DF74-1048-292F-2824-F4C0F07B88AE}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1711,7 +1747,7 @@
         <xdr:cNvPr id="10" name="image2.png" title="Imagem">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5A21D065-F18E-49C1-BDED-7A055802AC65}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C366AC29-14C6-49F0-A8E5-3EC6921FD53C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1749,7 +1785,7 @@
         <xdr:cNvPr id="11" name="image1.png" title="Imagem">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FE12FF15-E61E-41F2-BF96-B14C2736DED0}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4AAA7A34-3E49-4D28-895C-B1BE49DBAC92}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1792,7 +1828,7 @@
         <xdr:cNvPr id="12" name="Imagem 11">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EFABF35D-23DD-4C80-9751-B1CF7F16AFAA}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C6374A08-3C29-445B-A26B-0F724D3F2C30}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2105,7 +2141,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A86770B7-42B2-43DE-B011-1619F3850E46}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B55C20BC-5C02-4C56-98D6-3A926DBF865A}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
@@ -2117,98 +2153,98 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="5" width="12.5703125" style="38"/>
-    <col min="6" max="6" width="2" style="38" customWidth="1"/>
-    <col min="7" max="16" width="13.42578125" style="38" customWidth="1"/>
-    <col min="17" max="16384" width="12.5703125" style="38"/>
+    <col min="1" max="5" width="12.5703125" style="40"/>
+    <col min="6" max="6" width="2" style="40" customWidth="1"/>
+    <col min="7" max="16" width="13.42578125" style="40" customWidth="1"/>
+    <col min="17" max="16384" width="12.5703125" style="40"/>
   </cols>
   <sheetData>
     <row r="1" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F1" s="37"/>
+      <c r="F1" s="39"/>
     </row>
     <row r="2" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F2" s="37"/>
+      <c r="F2" s="39"/>
     </row>
     <row r="3" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F3" s="37"/>
+      <c r="F3" s="39"/>
     </row>
     <row r="4" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F4" s="37"/>
+      <c r="F4" s="39"/>
     </row>
     <row r="5" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F5" s="37"/>
+      <c r="F5" s="39"/>
     </row>
     <row r="6" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F6" s="37"/>
+      <c r="F6" s="39"/>
     </row>
     <row r="7" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F7" s="37"/>
+      <c r="F7" s="39"/>
     </row>
     <row r="8" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F8" s="37"/>
+      <c r="F8" s="39"/>
     </row>
     <row r="9" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F9" s="37"/>
+      <c r="F9" s="39"/>
     </row>
     <row r="10" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F10" s="37"/>
+      <c r="F10" s="39"/>
     </row>
     <row r="11" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F11" s="37"/>
+      <c r="F11" s="39"/>
     </row>
     <row r="12" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F12" s="37"/>
+      <c r="F12" s="39"/>
     </row>
     <row r="13" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F13" s="37"/>
+      <c r="F13" s="39"/>
     </row>
     <row r="14" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F14" s="37"/>
+      <c r="F14" s="39"/>
     </row>
     <row r="15" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F15" s="37"/>
+      <c r="F15" s="39"/>
     </row>
     <row r="16" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F16" s="37"/>
+      <c r="F16" s="39"/>
     </row>
     <row r="17" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F17" s="37"/>
+      <c r="F17" s="39"/>
     </row>
     <row r="18" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F18" s="37"/>
+      <c r="F18" s="39"/>
     </row>
     <row r="19" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F19" s="37"/>
+      <c r="F19" s="39"/>
     </row>
     <row r="20" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F20" s="37"/>
+      <c r="F20" s="39"/>
     </row>
     <row r="21" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F21" s="37"/>
+      <c r="F21" s="39"/>
     </row>
     <row r="22" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F22" s="37"/>
+      <c r="F22" s="39"/>
     </row>
     <row r="23" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F23" s="37"/>
+      <c r="F23" s="39"/>
     </row>
     <row r="24" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F24" s="37"/>
+      <c r="F24" s="39"/>
     </row>
     <row r="25" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F25" s="37"/>
+      <c r="F25" s="39"/>
     </row>
     <row r="26" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F26" s="37"/>
+      <c r="F26" s="39"/>
     </row>
     <row r="27" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F27" s="37"/>
+      <c r="F27" s="39"/>
     </row>
     <row r="28" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F28" s="37"/>
+      <c r="F28" s="39"/>
     </row>
     <row r="29" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F29" s="37"/>
+      <c r="F29" s="39"/>
     </row>
   </sheetData>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
@@ -7295,4 +7331,44 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="26.42578125" customWidth="1"/>
+    <col min="2" max="2" width="15.85546875" customWidth="1"/>
+    <col min="3" max="3" width="88.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="37" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="37" t="s">
+        <v>355</v>
+      </c>
+      <c r="C1" s="37" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="38" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="38" t="s">
+        <v>357</v>
+      </c>
+      <c r="C2" s="38" t="s">
+        <v>358</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>